<commit_message>
Atualização - Lista de variáveis - Classes A
</commit_message>
<xml_diff>
--- a/Atividade 2 - Lista de variáveis_A.xlsx
+++ b/Atividade 2 - Lista de variáveis_A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="15156" windowHeight="7992" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="15156" windowHeight="7992" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="View" sheetId="7" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="37">
   <si>
     <t>Class</t>
   </si>
@@ -33,258 +33,12 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Barber</t>
-  </si>
-  <si>
-    <t>Barbeiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> // Constant that receives a invalid name of a barber</t>
-  </si>
-  <si>
-    <t>// Constant that receives a blank name of a barber</t>
-  </si>
-  <si>
-    <t>// Constant that receives a invalid telephone of a barber</t>
-  </si>
-  <si>
-    <t>// Constant that receives a blank telephone of a barber</t>
-  </si>
-  <si>
-    <t>// Constant that receives a invalid chair of a barber</t>
-  </si>
-  <si>
-    <t>// Constant that receives a blank chair of a barber</t>
-  </si>
-  <si>
-    <t>// Receives the temporary name of a barber</t>
-  </si>
-  <si>
-    <t>// Receives the  name of a barber</t>
-  </si>
-  <si>
-    <t>// Receives the Rg of a barber</t>
-  </si>
-  <si>
-    <t>// Receives the telephone of a barber</t>
-  </si>
-  <si>
-    <t>// Receives the chair of a barber</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NOME_INVALIDO </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NOME_BRANCO </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CPF_INVALIDO </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CPF_BRANCO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RG_BRANCO </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RG_INVALIDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TELEFONE_INVALIDO </t>
-  </si>
-  <si>
-    <t>CADEIRA_INVALIDA</t>
-  </si>
-  <si>
-    <t>// Constant that receives a invalid Cpf (cadastro de pessoa física, in portuguese) of a barber</t>
-  </si>
-  <si>
-    <t>// Constant that receives a blank Cpf (cadastro de pessoa física, in portuguese) of a barber</t>
-  </si>
-  <si>
-    <t>// Constant that receives a blank rg (registro geral, in portuguese) of a barber</t>
-  </si>
-  <si>
-    <t>// Constant that receives a invalid rg (registro geral, in portuguese)  of a barber</t>
-  </si>
-  <si>
-    <t>// Receives the Cpf (cadastro de pessoa física, in portuguese) of a barber</t>
-  </si>
-  <si>
-    <t>TELEFONE_BRANCO</t>
-  </si>
-  <si>
-    <t>CADEIRA_BRANCO</t>
-  </si>
-  <si>
-    <t>tempNome</t>
-  </si>
-  <si>
     <t>nome</t>
   </si>
   <si>
-    <t>cpf</t>
-  </si>
-  <si>
-    <t>rg</t>
-  </si>
-  <si>
-    <t>telefone</t>
-  </si>
-  <si>
-    <t>cadeira</t>
-  </si>
-  <si>
-    <t>INVALID_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  BLANK_CPF </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  BLANK_RG </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  INVALID_RG </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> INVALID_TELEPHONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  BLANK_TELEPHONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> INVALID_CHAIR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  BLANK_CHAIR </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> temporaryName</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> barberName</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> barberCpf</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> barberRg</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> barberTelephone</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> barberChair </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  BLANK_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  INVALID_CPF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> // Auxiliary variables to check Cpf (cadastro de pessoa física, in portuguese)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d2  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">digito1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">digito2 </t>
-  </si>
-  <si>
-    <t>// Variables used to represent the last two digits of a Cpf(cadastro de pessoa física, in portuguese)</t>
-  </si>
-  <si>
-    <t>resto</t>
-  </si>
-  <si>
-    <t>// Auxiliary variable to check Cpf (cadastro de pessoa física, in portuguese)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">digitoCPF;  </t>
-  </si>
-  <si>
-    <t>// Receives the current digit of the Cpf (cadastro de pessoa física, in portuguese)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String result; </t>
-  </si>
-  <si>
-    <t>// No suggestion</t>
-  </si>
-  <si>
-    <t>// Receives the last two digits of a Cpf(cadastro de pessoa física, in portuguese</t>
-  </si>
-  <si>
-    <t>nCount;</t>
-  </si>
-  <si>
-    <t>// Variable used to walk through the digits of cpf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">auxiliary1                                </t>
-  </si>
-  <si>
-    <t>auxiliary2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> penultimateDigit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> lastDigit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> rest </t>
-  </si>
-  <si>
-    <t>cpfDigit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> currentDigit</t>
-  </si>
-  <si>
-    <t>validarCpf</t>
-  </si>
-  <si>
-    <t>validateCpf</t>
-  </si>
-  <si>
-    <t>verific</t>
-  </si>
-  <si>
-    <t>// Receives the last two digits of a Cpf(cadastro de pessoa física, in portuguese)</t>
-  </si>
-  <si>
-    <t>BarbeiroDAO</t>
-  </si>
-  <si>
-    <t>DAOBarber</t>
-  </si>
-  <si>
     <t>incluir</t>
   </si>
   <si>
-    <t>includeBarber</t>
-  </si>
-  <si>
-    <t>barber</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> // Barber class instance</t>
-  </si>
-  <si>
-    <t>barbeiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> nome</t>
-  </si>
-  <si>
     <t>barberName</t>
   </si>
   <si>
@@ -303,18 +57,9 @@
     <t>alterar</t>
   </si>
   <si>
-    <t>changeBarber</t>
-  </si>
-  <si>
     <t>rs</t>
   </si>
   <si>
-    <t>instanceResult</t>
-  </si>
-  <si>
-    <t>//ResultSet interface instance</t>
-  </si>
-  <si>
     <t>AgendaController</t>
   </si>
   <si>
@@ -366,23 +111,32 @@
     <t>Variable name suggestion</t>
   </si>
   <si>
-    <t>instance</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Class variable</t>
-  </si>
-  <si>
-    <t>PhonebookController</t>
+    <t>ResultBarber</t>
+  </si>
+  <si>
+    <t>pesquisarPorDataEBarbeiro</t>
+  </si>
+  <si>
+    <t>searchForDateAndBarber</t>
+  </si>
+  <si>
+    <t>instanceStatement</t>
+  </si>
+  <si>
+    <t>//Instance the java.sql.preparedStatement</t>
+  </si>
+  <si>
+    <t>pst</t>
+  </si>
+  <si>
+    <t>RelatorioDAO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,6 +154,12 @@
     </font>
     <font>
       <sz val="7"/>
+      <color rgb="FF3E454C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF3E454C"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -740,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -785,9 +545,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -825,6 +582,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -876,9 +636,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -888,6 +645,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,25 +967,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="35" t="s">
+      <c r="F1" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="34" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1693,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1709,301 +1471,187 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.600000000000001" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="35" t="s">
+      <c r="F1" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A2" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>4</v>
-      </c>
+      <c r="A2" s="39"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="12"/>
       <c r="D2" s="8"/>
-      <c r="E2" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="40"/>
       <c r="B3" s="37"/>
       <c r="C3" s="11"/>
-      <c r="E3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="40"/>
       <c r="B4" s="37"/>
       <c r="C4" s="11"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="A5" s="40"/>
       <c r="B5" s="37"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
       <c r="A6" s="40"/>
       <c r="B6" s="37"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1">
       <c r="A7" s="40"/>
       <c r="B7" s="37"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1">
       <c r="A8" s="40"/>
       <c r="B8" s="37"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1">
       <c r="A9" s="40"/>
       <c r="B9" s="37"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1">
       <c r="A10" s="40"/>
       <c r="B10" s="37"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1">
       <c r="A11" s="40"/>
       <c r="B11" s="37"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1">
       <c r="A12" s="40"/>
       <c r="B12" s="37"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1">
       <c r="A13" s="40"/>
       <c r="B13" s="37"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1">
       <c r="A14" s="40"/>
       <c r="B14" s="37"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1">
       <c r="A15" s="40"/>
       <c r="B15" s="37"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1">
       <c r="A16" s="40"/>
       <c r="B16" s="37"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1">
       <c r="A17" s="40"/>
       <c r="B17" s="37"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="40"/>
       <c r="B18" s="37"/>
-      <c r="C18" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" s="48" t="s">
-        <v>55</v>
-      </c>
+      <c r="C18" s="45"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="48"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="40"/>
       <c r="B19" s="37"/>
       <c r="C19" s="46"/>
       <c r="D19" s="43"/>
-      <c r="E19" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>70</v>
-      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="49"/>
     </row>
     <row r="20" spans="1:7">
@@ -2011,27 +1659,17 @@
       <c r="B20" s="37"/>
       <c r="C20" s="46"/>
       <c r="D20" s="43"/>
-      <c r="E20" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" s="50" t="s">
-        <v>59</v>
-      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="50"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="40"/>
       <c r="B21" s="37"/>
       <c r="C21" s="46"/>
       <c r="D21" s="43"/>
-      <c r="E21" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="51"/>
     </row>
     <row r="22" spans="1:7">
@@ -2039,75 +1677,44 @@
       <c r="B22" s="37"/>
       <c r="C22" s="46"/>
       <c r="D22" s="43"/>
-      <c r="E22" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="40"/>
       <c r="B23" s="37"/>
       <c r="C23" s="46"/>
       <c r="D23" s="43"/>
-      <c r="E23" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>63</v>
-      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="40"/>
       <c r="B24" s="37"/>
       <c r="C24" s="46"/>
       <c r="D24" s="43"/>
-      <c r="E24" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="40"/>
       <c r="B25" s="37"/>
       <c r="C25" s="46"/>
       <c r="D25" s="43"/>
-      <c r="E25" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>68</v>
-      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="41"/>
       <c r="B26" s="38"/>
       <c r="C26" s="47"/>
       <c r="D26" s="44"/>
-      <c r="E26" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" t="s">
-        <v>65</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>79</v>
-      </c>
+      <c r="E26" s="7"/>
+      <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="3"/>
@@ -2190,346 +1797,370 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A2" sqref="A2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="40.44140625" style="34" customWidth="1"/>
-    <col min="2" max="2" width="39.5546875" style="34" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" style="34" customWidth="1"/>
-    <col min="4" max="4" width="36.109375" style="34" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" style="34" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="34" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.44140625" style="33" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" style="33" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" style="33" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" style="33" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="35" t="s">
+      <c r="F1" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>118</v>
+      <c r="A2" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>15</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>117</v>
+        <v>5</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -2539,7 +2170,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A2" sqref="A2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2555,99 +2186,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="35" t="s">
+      <c r="F1" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="34" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>86</v>
+    <row r="2" spans="1:7" ht="15.6">
+      <c r="A2" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>12</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>85</v>
+        <v>33</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="52" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>87</v>
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="23" t="s">
+        <v>35</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="25" t="s">
-        <v>90</v>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="24" t="s">
+        <v>8</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>91</v>
+        <v>9</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="56"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>97</v>
-      </c>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="6"/>
@@ -2903,10 +2521,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A2:A5"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2936,19 +2554,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>113</v>
+        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>114</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -2959,8 +2577,8 @@
       <c r="B2" s="52"/>
       <c r="C2" s="7"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7">
@@ -2975,9 +2593,9 @@
     <row r="4" spans="1:7">
       <c r="A4" s="52"/>
       <c r="B4" s="52"/>
-      <c r="C4" s="22"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="24"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
@@ -2986,7 +2604,7 @@
       <c r="B5" s="52"/>
       <c r="C5" s="52"/>
       <c r="D5" s="52"/>
-      <c r="E5" s="24"/>
+      <c r="E5" s="23"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
@@ -3011,152 +2629,152 @@
     <row r="8" spans="1:7">
       <c r="A8" s="52"/>
       <c r="B8" s="52"/>
-      <c r="C8" s="22"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="24"/>
+      <c r="E8" s="23"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="54"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="22"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="24"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="55"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="27"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="55"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="28"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="24"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="55"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="55"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="24"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="55"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="55"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="24"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="55"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="56"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="24"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="54" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18" s="54" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>104</v>
+      <c r="A18" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>19</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>102</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="55"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>103</v>
+      <c r="A19" s="54"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>105</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="56"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>106</v>
+      <c r="A20" s="55"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>108</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3295,7 +2913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
@@ -3309,25 +2927,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="35" t="s">
+      <c r="F1" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="34" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização - Lista de Variáveis - Classe A
Classe Agenda
</commit_message>
<xml_diff>
--- a/Atividade 2 - Lista de variáveis_A.xlsx
+++ b/Atividade 2 - Lista de variáveis_A.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="51">
   <si>
     <t>Class</t>
   </si>
@@ -130,6 +130,48 @@
   </si>
   <si>
     <t>RelatorioDAO</t>
+  </si>
+  <si>
+    <t>Agenda</t>
+  </si>
+  <si>
+    <t>Phonebook</t>
+  </si>
+  <si>
+    <t>receivesAgenda</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>//Receives the name for phonebook</t>
+  </si>
+  <si>
+    <t>telefone</t>
+  </si>
+  <si>
+    <t>//Receives the number of phone for phonebook</t>
+  </si>
+  <si>
+    <t>descrição</t>
+  </si>
+  <si>
+    <t>phonebookDs</t>
+  </si>
+  <si>
+    <t>//Receives the description for phonebook</t>
+  </si>
+  <si>
+    <t>getTempName</t>
+  </si>
+  <si>
+    <t>no sugestion</t>
+  </si>
+  <si>
+    <t>tempName</t>
+  </si>
+  <si>
+    <t>//Receives the variable for change the metod</t>
   </si>
 </sst>
 </file>
@@ -179,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -245,32 +287,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -475,10 +491,23 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color theme="3" tint="-0.249977111117893"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -486,21 +515,80 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right style="medium">
+        <color theme="3"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,24 +609,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -572,7 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -585,71 +663,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,25 +1069,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="30" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1456,7 +1558,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A2" sqref="A2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1471,248 +1573,285 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.600000000000001" thickBot="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A2" s="39"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="A2" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
-      <c r="A3" s="40"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="11"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="A5" s="40"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
-      <c r="A6" s="40"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="13"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1">
-      <c r="A7" s="40"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="13"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1">
-      <c r="A8" s="40"/>
-      <c r="B8" s="37"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="13"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1">
-      <c r="A9" s="40"/>
-      <c r="B9" s="37"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="14"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1">
-      <c r="A10" s="40"/>
-      <c r="B10" s="37"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="15"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1">
-      <c r="A11" s="40"/>
-      <c r="B11" s="37"/>
+      <c r="A11" s="47"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="16"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1">
-      <c r="A12" s="40"/>
-      <c r="B12" s="37"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="16"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1">
-      <c r="A13" s="40"/>
-      <c r="B13" s="37"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="48"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="16"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1">
-      <c r="A14" s="40"/>
-      <c r="B14" s="37"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="17"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1">
-      <c r="A15" s="40"/>
-      <c r="B15" s="37"/>
+      <c r="A15" s="47"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="13"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1">
-      <c r="A16" s="40"/>
-      <c r="B16" s="37"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="48"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1">
-      <c r="A17" s="40"/>
-      <c r="B17" s="37"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="13"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="40"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="42"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="48"/>
+      <c r="G18" s="39"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="40"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="43"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="49"/>
+      <c r="G19" s="40"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="40"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="43"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="50"/>
+      <c r="G20" s="41"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="40"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="43"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="51"/>
+      <c r="G21" s="42"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="40"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="43"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="40"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="43"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="52"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="40"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="43"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="40"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="43"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="52"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="41"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="44"/>
+      <c r="A26" s="53"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="56"/>
       <c r="E26" s="7"/>
       <c r="G26" s="7"/>
     </row>
@@ -1721,8 +1860,8 @@
       <c r="B27" s="5"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="17"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7">
@@ -1730,27 +1869,27 @@
       <c r="B28" s="5"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="13"/>
+      <c r="E28" s="9"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="18"/>
+      <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="3"/>
       <c r="B29" s="5"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="13"/>
+      <c r="E29" s="9"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="18"/>
+      <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="3"/>
       <c r="B30" s="5"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="13"/>
+      <c r="E30" s="9"/>
       <c r="F30" s="7"/>
-      <c r="G30" s="18"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="3"/>
@@ -1759,7 +1898,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="5"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="18"/>
+      <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="3"/>
@@ -1767,8 +1906,8 @@
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="3"/>
@@ -1776,17 +1915,17 @@
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B2:B26"/>
-    <mergeCell ref="A2:A26"/>
-    <mergeCell ref="D18:D26"/>
-    <mergeCell ref="C18:C26"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1802,55 +1941,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="40.44140625" style="33" customWidth="1"/>
-    <col min="2" max="2" width="39.5546875" style="33" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" style="33" customWidth="1"/>
-    <col min="4" max="4" width="36.109375" style="33" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" style="33" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.44140625" style="29" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" style="29" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" style="29" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" style="29" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="28" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="7" t="s">
@@ -1858,18 +1997,18 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="26" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="28" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -1877,15 +2016,15 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="35" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -1896,265 +2035,265 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2186,57 +2325,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.6">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="23" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="19" t="s">
         <v>35</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -2247,11 +2386,11 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="24" t="s">
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="20" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -2262,10 +2401,10 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="6"/>
@@ -2573,17 +2712,17 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
       <c r="C2" s="7"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="6"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -2591,148 +2730,148 @@
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="21"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="23"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="23"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="52"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="21"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="23"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="53"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="21"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="23"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="54"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="26"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="54"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="27"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="23"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="54"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="54"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="23"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="54"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="54"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="23"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="54"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="55"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="23"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="28" t="s">
         <v>19</v>
       </c>
       <c r="G18" s="7" t="s">
@@ -2740,18 +2879,18 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="54"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="26" t="s">
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="28" t="s">
         <v>18</v>
       </c>
       <c r="G19" s="7" t="s">
@@ -2759,15 +2898,15 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="55"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="29" t="s">
+      <c r="A20" s="45"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F20" s="7" t="s">
@@ -2927,25 +3066,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="30" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>